<commit_message>
modification de c9, validation des outputs jobs, todo: modif footprints condos + design rules checks
</commit_message>
<xml_diff>
--- a/POC/Altium/Project Outputs for POC_Marvin/Bill of Materials/Bill of Materials.xlsx
+++ b/POC/Altium/Project Outputs for POC_Marvin/Bill of Materials/Bill of Materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29880" windowHeight="11625"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15060" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="1" r:id="rId1"/>
@@ -743,14 +743,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>